<commit_message>
Report ng Itextcontext depenency in pom for reportn ng
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/tasks.xlsx
+++ b/src/test/resources/TestData/tasks.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madhubs\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11100" windowHeight="4065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="95">
   <si>
     <t>Sno</t>
   </si>
@@ -302,6 +298,15 @@
   </si>
   <si>
     <t>completed</t>
+  </si>
+  <si>
+    <t>itextcontext</t>
+  </si>
+  <si>
+    <t>log4j implementation</t>
+  </si>
+  <si>
+    <t>reportng</t>
   </si>
 </sst>
 </file>
@@ -691,7 +696,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,7 +857,9 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -862,7 +869,9 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -872,7 +881,9 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>

</xml_diff>